<commit_message>
[+] começo da tabulação
</commit_message>
<xml_diff>
--- a/teoria/pesquisa-bib-dissert.xlsx
+++ b/teoria/pesquisa-bib-dissert.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="52" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="83">
   <si>
     <t xml:space="preserve">ANO</t>
   </si>
@@ -34,7 +34,7 @@
     <t xml:space="preserve">SURVEY</t>
   </si>
   <si>
-    <t xml:space="preserve">IDIOMA</t>
+    <t xml:space="preserve">PT-BR</t>
   </si>
   <si>
     <t xml:space="preserve">ABORDAGEM</t>
@@ -49,21 +49,54 @@
     <t xml:space="preserve">TARGET</t>
   </si>
   <si>
-    <t xml:space="preserve">MELHORIAS</t>
+    <t xml:space="preserve">OBS</t>
   </si>
   <si>
     <t xml:space="preserve">Speech Emotion Recognition using Supervised Deep Recurrent System for Mental Health Monitoring</t>
   </si>
   <si>
+    <t xml:space="preserve"> -</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n</t>
+  </si>
+  <si>
+    <t xml:space="preserve">sup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cnn, rnn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mfcc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emo</t>
+  </si>
+  <si>
+    <t xml:space="preserve">domain fusion</t>
+  </si>
+  <si>
     <t xml:space="preserve">Depression Recognition using Remote Photoplethysmography from Facial Videos</t>
   </si>
   <si>
+    <t xml:space="preserve">-</t>
+  </si>
+  <si>
     <t xml:space="preserve">Accurate Emotion Strength Assessment for Seen and Unseen Speech Based on Data-Driven Deep Learning</t>
   </si>
   <si>
+    <t xml:space="preserve">unsup sup</t>
+  </si>
+  <si>
+    <t xml:space="preserve">emo, str</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emotional Speaker Identification using a Novel Capsule Nets Model</t>
   </si>
   <si>
+    <t xml:space="preserve">cnn, dnn</t>
+  </si>
+  <si>
     <t xml:space="preserve">MEL Spectrogram</t>
   </si>
   <si>
@@ -73,46 +106,106 @@
     <t xml:space="preserve">Automated Sex Classification of Children's Voices and Changes in Differentiating Factors with Age</t>
   </si>
   <si>
+    <t xml:space="preserve">rf</t>
+  </si>
+  <si>
+    <t xml:space="preserve">freqs</t>
+  </si>
+  <si>
     <t xml:space="preserve">Language Independent Emotion Quantification using Non linear Modelling of Speech</t>
   </si>
   <si>
     <t xml:space="preserve">Voice Conversion Based on Cross-Domain Features Using Variational Auto Encoders</t>
   </si>
   <si>
+    <t xml:space="preserve">ae</t>
+  </si>
+  <si>
     <t xml:space="preserve">A Fine-tuned Wav2vec 2.0/HuBERT Benchmark For Speech Emotion Recognition, Speaker Verification and Spoken Language Understanding</t>
   </si>
   <si>
+    <t xml:space="preserve">cnn, enc</t>
+  </si>
+  <si>
     <t xml:space="preserve">Improving Automatic Emotion Recognition from speech using Rhythm and Temporal feature</t>
   </si>
   <si>
+    <t xml:space="preserve">dnn</t>
+  </si>
+  <si>
     <t xml:space="preserve">DEEP: Uma arquitetura para reconhecer emoção com base no espectro sonoro da voz de falantes da língua portuguesa</t>
   </si>
   <si>
+    <t xml:space="preserve">?</t>
+  </si>
+  <si>
+    <t xml:space="preserve">s</t>
+  </si>
+  <si>
+    <t xml:space="preserve">pros, croma, mfcc</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modelos especialistas</t>
+  </si>
+  <si>
     <t xml:space="preserve">A Knowledge-Based Recommendation System That Includes Sentiment Analysis and Deep Learning</t>
   </si>
   <si>
+    <t xml:space="preserve">nível de estresse</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emotion intensity detection for social media data</t>
   </si>
   <si>
+    <t xml:space="preserve">tweets</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emotion Detection and Analysis on Social Media</t>
   </si>
   <si>
     <t xml:space="preserve">The paradoxical role of emotional intensity in the perception of vocal affect</t>
   </si>
   <si>
+    <t xml:space="preserve">sobre intensidade</t>
+  </si>
+  <si>
     <t xml:space="preserve">Human Emotion Recognition: Review of Sensors and Methods </t>
   </si>
   <si>
+    <t xml:space="preserve">sensores para abordagens com dados fisiológicos</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emotion Intensity and its Control for Emotional Voice Conversion</t>
   </si>
   <si>
+    <t xml:space="preserve">mfcc, speech2text</t>
+  </si>
+  <si>
     <t xml:space="preserve">Emotional Intensity Level Analysis of Speech Emotional Intensity Estimation</t>
   </si>
   <si>
+    <t xml:space="preserve">svm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mfcc, spectral, pitch</t>
+  </si>
+  <si>
     <t xml:space="preserve">Recognition of Emotion with Intensity from Speech Signal Using 3D Transformed Feature and Deep Learning</t>
   </si>
   <si>
+    <t xml:space="preserve">mfcc,sfft, chroma</t>
+  </si>
+  <si>
+    <t xml:space="preserve">mais de um modelo proposto</t>
+  </si>
+  <si>
     <t xml:space="preserve">Brazilian Portuguese emotional speech corpus analysis</t>
+  </si>
+  <si>
+    <t xml:space="preserve">svm, dnn</t>
+  </si>
+  <si>
+    <t xml:space="preserve">utiliza modelos tradicionais</t>
   </si>
   <si>
     <t xml:space="preserve">END-TO-END SPEECH RECOGNITION APPLIED TO BRAZILIAN PORTUGUESE USING DEEP LEARNING</t>
@@ -185,7 +278,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="General"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -224,6 +317,13 @@
     <font>
       <sz val="12"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FFC9211E"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
@@ -296,7 +396,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -319,6 +419,10 @@
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="left" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="6" fillId="4" borderId="1" xfId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="false">
@@ -400,7 +504,7 @@
       <rgbColor rgb="FF339966"/>
       <rgbColor rgb="FF003300"/>
       <rgbColor rgb="FF333300"/>
-      <rgbColor rgb="FF993300"/>
+      <rgbColor rgb="FFC9211E"/>
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
@@ -417,7 +521,7 @@
   <dimension ref="A1:J206"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="75" zoomScaleNormal="75" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H28" activeCellId="0" sqref="H28"/>
+      <selection pane="topLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="15" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -425,10 +529,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="8.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="143.48"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="10.09"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="5" min="4" style="1" width="11.52"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="10.46"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="8.23"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="16.39"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.34"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="26.31"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="13.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="26.32"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="11.52"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="84.11"/>
     <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1024" min="11" style="1" width="11.52"/>
@@ -467,333 +572,683 @@
       </c>
     </row>
     <row r="2" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="3"/>
+      <c r="A2" s="3" t="n">
+        <v>2022</v>
+      </c>
       <c r="B2" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3"/>
-      <c r="J2" s="3"/>
+      <c r="C2" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I2" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J2" s="3" t="s">
+        <v>17</v>
+      </c>
     </row>
     <row r="3" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="5"/>
+      <c r="A3" s="5" t="n">
+        <v>2022</v>
+      </c>
       <c r="B3" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="5"/>
-      <c r="D3" s="5"/>
-      <c r="E3" s="5"/>
-      <c r="F3" s="5"/>
-      <c r="G3" s="5"/>
-      <c r="H3" s="5"/>
-      <c r="I3" s="5"/>
-      <c r="J3" s="5"/>
+        <v>18</v>
+      </c>
+      <c r="C3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="E3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I3" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="4" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="3"/>
+      <c r="A4" s="3" t="n">
+        <v>2022</v>
+      </c>
       <c r="B4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="C4" s="3" t="n">
+        <v>1</v>
+      </c>
+      <c r="D4" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="3"/>
-      <c r="D4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="F4" s="3"/>
-      <c r="G4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="I4" s="3"/>
-      <c r="J4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="G4" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I4" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J4" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="5" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="5"/>
-      <c r="B5" s="6" t="s">
+      <c r="A5" s="5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="C5" s="5" t="n">
+        <v>4</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E5" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F5" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-      <c r="G5" s="5"/>
-      <c r="H5" s="5"/>
-      <c r="I5" s="5"/>
-      <c r="J5" s="5"/>
+      <c r="G5" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H5" s="5" t="s">
+        <v>15</v>
+      </c>
+      <c r="I5" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="6" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="3"/>
+      <c r="A6" s="3" t="s">
+        <v>19</v>
+      </c>
       <c r="B6" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="I6" s="3"/>
-      <c r="J6" s="3"/>
+        <v>25</v>
+      </c>
+      <c r="C6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="F6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I6" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J6" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="7" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="5"/>
-      <c r="B7" s="6" t="s">
+      <c r="A7" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B7" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E7" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F7" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H7" s="5" t="s">
         <v>15</v>
       </c>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-      <c r="G7" s="5"/>
-      <c r="H7" s="5"/>
-      <c r="I7" s="5"/>
-      <c r="J7" s="5"/>
+      <c r="I7" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J7" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="8" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="3"/>
+      <c r="A8" s="3" t="n">
+        <v>2022</v>
+      </c>
       <c r="B8" s="4" t="s">
-        <v>16</v>
-      </c>
-      <c r="C8" s="3"/>
-      <c r="D8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="F8" s="3"/>
-      <c r="G8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="I8" s="3"/>
-      <c r="J8" s="3"/>
+        <v>27</v>
+      </c>
+      <c r="C8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E8" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F8" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G8" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="I8" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J8" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="5"/>
-      <c r="B9" s="6" t="s">
-        <v>17</v>
-      </c>
-      <c r="C9" s="5"/>
-      <c r="D9" s="5"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-      <c r="G9" s="5"/>
-      <c r="H9" s="5"/>
-      <c r="I9" s="5"/>
-      <c r="J9" s="5"/>
+      <c r="A9" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B9" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="C9" s="5" t="n">
+        <v>1</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E9" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I9" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J9" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="3" t="n">
         <v>2018</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>18</v>
+        <v>31</v>
       </c>
       <c r="C10" s="3" t="n">
         <v>39</v>
       </c>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
-      <c r="F10" s="3"/>
-      <c r="G10" s="3"/>
-      <c r="H10" s="3"/>
-      <c r="I10" s="3"/>
-      <c r="J10" s="3"/>
+      <c r="D10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G10" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="H10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I10" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J10" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="5"/>
-      <c r="B11" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="5"/>
-      <c r="D11" s="5"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-      <c r="G11" s="5"/>
-      <c r="H11" s="5"/>
-      <c r="I11" s="5"/>
-      <c r="J11" s="5"/>
+      <c r="A11" s="5" t="n">
+        <v>2021</v>
+      </c>
+      <c r="B11" s="7" t="s">
+        <v>33</v>
+      </c>
+      <c r="C11" s="5" t="n">
+        <v>25</v>
+      </c>
+      <c r="D11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E11" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F11" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H11" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I11" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J11" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="3" t="n">
         <v>2013</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="C12" s="3" t="n">
         <v>35</v>
       </c>
-      <c r="D12" s="3"/>
-      <c r="E12" s="3"/>
-      <c r="F12" s="3"/>
-      <c r="G12" s="3"/>
-      <c r="H12" s="3"/>
-      <c r="I12" s="3"/>
-      <c r="J12" s="3"/>
-    </row>
-    <row r="13" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="7"/>
-      <c r="B13" s="8" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="7"/>
-      <c r="D13" s="5"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-      <c r="G13" s="5"/>
-      <c r="H13" s="5"/>
-      <c r="I13" s="5"/>
-      <c r="J13" s="5"/>
+      <c r="D12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E12" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F12" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G12" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="H12" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I12" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J12" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="8" t="n">
+        <v>2020</v>
+      </c>
+      <c r="B13" s="9" t="s">
+        <v>37</v>
+      </c>
+      <c r="C13" s="8" t="s">
+        <v>38</v>
+      </c>
+      <c r="D13" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E13" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="F13" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="H13" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="I13" s="5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J13" s="5" t="s">
+        <v>41</v>
+      </c>
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="3" t="n">
         <v>2018</v>
       </c>
       <c r="B14" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="C14" s="3" t="n">
+        <v>122</v>
+      </c>
+      <c r="D14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F14" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G14" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="H14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I14" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J14" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="5" t="n">
+        <v>2017</v>
+      </c>
+      <c r="B15" s="7" t="s">
+        <v>44</v>
+      </c>
+      <c r="C15" s="5" t="n">
+        <v>18</v>
+      </c>
+      <c r="D15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E15" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F15" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H15" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I15" s="5" t="s">
         <v>22</v>
       </c>
-      <c r="C14" s="3" t="n">
-        <v>115</v>
-      </c>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
-      <c r="I14" s="3"/>
-      <c r="J14" s="3"/>
-    </row>
-    <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="5"/>
-      <c r="B15" s="6" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="5"/>
-      <c r="D15" s="5"/>
-      <c r="E15" s="5"/>
-      <c r="F15" s="5"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="5"/>
-      <c r="I15" s="5"/>
-      <c r="J15" s="5"/>
+      <c r="J15" s="5" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="3" t="n">
         <v>2019</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>24</v>
+        <v>46</v>
       </c>
       <c r="C16" s="3" t="n">
-        <v>47</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
-      <c r="I16" s="3"/>
-      <c r="J16" s="3"/>
+        <v>49</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F16" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H16" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I16" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J16" s="3" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="5" t="n">
         <v>2021</v>
       </c>
-      <c r="B17" s="6" t="s">
-        <v>25</v>
+      <c r="B17" s="7" t="s">
+        <v>47</v>
       </c>
       <c r="C17" s="5" t="n">
-        <v>16</v>
-      </c>
-      <c r="D17" s="5"/>
-      <c r="E17" s="5"/>
-      <c r="F17" s="5"/>
-      <c r="G17" s="5"/>
-      <c r="H17" s="5"/>
-      <c r="I17" s="5"/>
-      <c r="J17" s="5"/>
+        <v>20</v>
+      </c>
+      <c r="D17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E17" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="G17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="I17" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J17" s="5" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="3" t="n">
         <v>2020</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>26</v>
+        <v>49</v>
       </c>
       <c r="C18" s="3" t="n">
-        <v>204</v>
-      </c>
-      <c r="D18" s="3"/>
-      <c r="E18" s="3"/>
-      <c r="F18" s="3"/>
-      <c r="G18" s="3"/>
-      <c r="H18" s="3"/>
-      <c r="I18" s="3"/>
-      <c r="J18" s="3"/>
+        <v>219</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="G18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="I18" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J18" s="3" t="s">
+        <v>50</v>
+      </c>
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="5" t="n">
         <v>2022</v>
       </c>
-      <c r="B19" s="6" t="s">
-        <v>27</v>
+      <c r="B19" s="7" t="s">
+        <v>51</v>
       </c>
       <c r="C19" s="5" t="n">
-        <v>8</v>
-      </c>
-      <c r="D19" s="5"/>
-      <c r="E19" s="5"/>
-      <c r="F19" s="5"/>
-      <c r="G19" s="5"/>
-      <c r="H19" s="5"/>
-      <c r="I19" s="5"/>
-      <c r="J19" s="5"/>
+        <v>10</v>
+      </c>
+      <c r="D19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E19" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F19" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H19" s="5" t="s">
+        <v>52</v>
+      </c>
+      <c r="I19" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J19" s="5" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="3"/>
+      <c r="A20" s="3" t="n">
+        <v>2021</v>
+      </c>
       <c r="B20" s="4" t="s">
-        <v>28</v>
-      </c>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
-      <c r="F20" s="3"/>
-      <c r="G20" s="3"/>
-      <c r="H20" s="3"/>
-      <c r="I20" s="3"/>
-      <c r="J20" s="3"/>
+        <v>53</v>
+      </c>
+      <c r="C20" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="F20" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G20" s="3" t="s">
+        <v>54</v>
+      </c>
+      <c r="H20" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="I20" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J20" s="3" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="5"/>
-      <c r="B21" s="6" t="s">
-        <v>29</v>
-      </c>
-      <c r="C21" s="5"/>
-      <c r="D21" s="5"/>
-      <c r="E21" s="5"/>
-      <c r="F21" s="5"/>
-      <c r="G21" s="5"/>
-      <c r="H21" s="5"/>
-      <c r="I21" s="5"/>
-      <c r="J21" s="5"/>
+      <c r="A21" s="5" t="n">
+        <v>2022</v>
+      </c>
+      <c r="B21" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="C21" s="5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="E21" s="5" t="s">
+        <v>12</v>
+      </c>
+      <c r="F21" s="5" t="s">
+        <v>13</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>14</v>
+      </c>
+      <c r="H21" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="I21" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="J21" s="5" t="s">
+        <v>58</v>
+      </c>
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="3"/>
+      <c r="A22" s="3" t="n">
+        <v>2021</v>
+      </c>
       <c r="B22" s="4" t="s">
-        <v>30</v>
-      </c>
-      <c r="C22" s="3"/>
-      <c r="D22" s="3"/>
-      <c r="E22" s="3"/>
-      <c r="F22" s="3"/>
-      <c r="G22" s="3"/>
-      <c r="H22" s="3"/>
-      <c r="I22" s="3"/>
-      <c r="J22" s="3"/>
+        <v>59</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="D22" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="E22" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="F22" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="G22" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="H22" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="I22" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="J22" s="3" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="5" t="n">
         <v>2017</v>
       </c>
-      <c r="B23" s="6" t="s">
-        <v>31</v>
+      <c r="B23" s="7" t="s">
+        <v>62</v>
       </c>
       <c r="C23" s="5" t="n">
         <v>13</v>
@@ -809,7 +1264,7 @@
     <row r="24" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="3"/>
       <c r="B24" s="4" t="s">
-        <v>32</v>
+        <v>63</v>
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
@@ -822,8 +1277,8 @@
     </row>
     <row r="25" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="5"/>
-      <c r="B25" s="6" t="s">
-        <v>33</v>
+      <c r="B25" s="7" t="s">
+        <v>64</v>
       </c>
       <c r="C25" s="5"/>
       <c r="D25" s="5"/>
@@ -837,7 +1292,7 @@
     <row r="26" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="3"/>
       <c r="B26" s="4" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="C26" s="3"/>
       <c r="D26" s="3"/>
@@ -850,8 +1305,8 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="5"/>
-      <c r="B27" s="6" t="s">
-        <v>35</v>
+      <c r="B27" s="7" t="s">
+        <v>66</v>
       </c>
       <c r="C27" s="5"/>
       <c r="D27" s="5"/>
@@ -865,7 +1320,7 @@
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="3"/>
       <c r="B28" s="4" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
@@ -880,8 +1335,8 @@
       <c r="A29" s="5" t="n">
         <v>2019</v>
       </c>
-      <c r="B29" s="6" t="s">
-        <v>37</v>
+      <c r="B29" s="7" t="s">
+        <v>68</v>
       </c>
       <c r="C29" s="5" t="n">
         <v>24</v>
@@ -897,7 +1352,7 @@
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="3"/>
       <c r="B30" s="4" t="s">
-        <v>38</v>
+        <v>69</v>
       </c>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -910,8 +1365,8 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="5"/>
-      <c r="B31" s="6" t="s">
-        <v>39</v>
+      <c r="B31" s="7" t="s">
+        <v>70</v>
       </c>
       <c r="C31" s="5"/>
       <c r="D31" s="5"/>
@@ -925,7 +1380,7 @@
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="3"/>
       <c r="B32" s="4" t="s">
-        <v>40</v>
+        <v>71</v>
       </c>
       <c r="C32" s="3"/>
       <c r="D32" s="3"/>
@@ -940,8 +1395,8 @@
       <c r="A33" s="5" t="n">
         <v>2021</v>
       </c>
-      <c r="B33" s="6" t="s">
-        <v>41</v>
+      <c r="B33" s="7" t="s">
+        <v>72</v>
       </c>
       <c r="C33" s="5" t="n">
         <v>76</v>
@@ -957,7 +1412,7 @@
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="3"/>
       <c r="B34" s="4" t="s">
-        <v>42</v>
+        <v>73</v>
       </c>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -972,8 +1427,8 @@
       <c r="A35" s="5" t="n">
         <v>2018</v>
       </c>
-      <c r="B35" s="6" t="s">
-        <v>43</v>
+      <c r="B35" s="7" t="s">
+        <v>74</v>
       </c>
       <c r="C35" s="5" t="n">
         <v>48</v>
@@ -989,7 +1444,7 @@
     <row r="36" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="3"/>
       <c r="B36" s="4" t="s">
-        <v>44</v>
+        <v>75</v>
       </c>
       <c r="C36" s="3"/>
       <c r="D36" s="3"/>
@@ -1004,8 +1459,8 @@
       <c r="A37" s="5" t="n">
         <v>2020</v>
       </c>
-      <c r="B37" s="6" t="s">
-        <v>45</v>
+      <c r="B37" s="7" t="s">
+        <v>76</v>
       </c>
       <c r="C37" s="5" t="n">
         <v>4</v>
@@ -1023,7 +1478,7 @@
         <v>2021</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>46</v>
+        <v>77</v>
       </c>
       <c r="C38" s="3" t="n">
         <v>18</v>
@@ -1038,8 +1493,8 @@
     </row>
     <row r="39" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="5"/>
-      <c r="B39" s="6" t="s">
-        <v>47</v>
+      <c r="B39" s="7" t="s">
+        <v>78</v>
       </c>
       <c r="C39" s="5"/>
       <c r="D39" s="5"/>
@@ -1055,7 +1510,7 @@
         <v>2012</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>48</v>
+        <v>79</v>
       </c>
       <c r="C40" s="3" t="n">
         <v>543</v>
@@ -1068,12 +1523,12 @@
       <c r="I40" s="3"/>
       <c r="J40" s="3"/>
     </row>
-    <row r="41" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="41" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="5" t="n">
         <v>2019</v>
       </c>
-      <c r="B41" s="8" t="s">
-        <v>49</v>
+      <c r="B41" s="9" t="s">
+        <v>80</v>
       </c>
       <c r="C41" s="5" t="n">
         <v>201</v>
@@ -1086,12 +1541,12 @@
       <c r="I41" s="5"/>
       <c r="J41" s="5"/>
     </row>
-    <row r="42" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="42" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="3" t="n">
         <v>2020</v>
       </c>
-      <c r="B42" s="9" t="s">
-        <v>50</v>
+      <c r="B42" s="10" t="s">
+        <v>81</v>
       </c>
       <c r="C42" s="3" t="n">
         <v>55</v>
@@ -1104,12 +1559,12 @@
       <c r="I42" s="3"/>
       <c r="J42" s="3"/>
     </row>
-    <row r="43" customFormat="false" ht="15.9" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="43" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="5" t="n">
         <v>2015</v>
       </c>
-      <c r="B43" s="8" t="s">
-        <v>51</v>
+      <c r="B43" s="9" t="s">
+        <v>82</v>
       </c>
       <c r="C43" s="5" t="n">
         <v>63</v>

</xml_diff>